<commit_message>
change sample format of department and designation csv/xlsx
</commit_message>
<xml_diff>
--- a/src/assets/formats/department.xlsx
+++ b/src/assets/formats/department.xlsx
@@ -22,18 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Testing</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -43,7 +37,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -52,14 +46,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -88,14 +74,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -367,7 +350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -375,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -389,26 +372,14 @@
     <col min="4" max="4" width="18.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:1" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix sheet name of designation and department xlsx
</commit_message>
<xml_diff>
--- a/src/assets/formats/department.xlsx
+++ b/src/assets/formats/department.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="-29475" yWindow="-8700" windowWidth="25605" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Employees" sheetId="1" r:id="rId1"/>
+    <sheet name="Departments" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -361,7 +361,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>

</xml_diff>

<commit_message>
fix format of department sample format file
</commit_message>
<xml_diff>
--- a/src/assets/formats/department.xlsx
+++ b/src/assets/formats/department.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="-29475" yWindow="-8700" windowWidth="25605" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Departments" sheetId="1" r:id="rId1"/>
+    <sheet name="Department" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
@@ -350,7 +350,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>